<commit_message>
EPBDS-6033 Add tests for length(T[])
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/Arrays.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/Arrays.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="24915" windowHeight="10995" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="24915" windowHeight="10995" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="isEmpty" sheetId="6" r:id="rId1"/>
@@ -14,13 +14,14 @@
     <sheet name="contains" sheetId="1" r:id="rId5"/>
     <sheet name="containsArrays" sheetId="2" r:id="rId6"/>
     <sheet name="containsAny" sheetId="5" r:id="rId7"/>
+    <sheet name="length" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2381" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2629" uniqueCount="453">
   <si>
     <r>
       <t xml:space="preserve">Method boolean </t>
@@ -2349,6 +2350,186 @@
   </si>
   <si>
     <t>t,t,f,,t,f</t>
+  </si>
+  <si>
+    <t>return length(mydata);</t>
+  </si>
+  <si>
+    <t>Method int lengthbyte(byte[] mydata)</t>
+  </si>
+  <si>
+    <t>Method int lengthByte(Byte[] mydata)</t>
+  </si>
+  <si>
+    <t>Method int lengthByteValue(ByteValue[] mydata)</t>
+  </si>
+  <si>
+    <t>Method int lengthshort(short[] mydata)</t>
+  </si>
+  <si>
+    <t>Method int lengthShort(Short[] mydata)</t>
+  </si>
+  <si>
+    <t>Method int lengthShortValue(ShortValue[] mydata)</t>
+  </si>
+  <si>
+    <t>Method int lengthint(int[] mydata)</t>
+  </si>
+  <si>
+    <t>Method int lengthInteger(Integer[] mydata)</t>
+  </si>
+  <si>
+    <t>Method int lengthIntValue(IntValue[] mydata)</t>
+  </si>
+  <si>
+    <t>Method int lengthlong(long[] mydata)</t>
+  </si>
+  <si>
+    <t>Method int lengthLong(Long[] mydata)</t>
+  </si>
+  <si>
+    <t>Method int lengthLongValue(LongValue[] mydata)</t>
+  </si>
+  <si>
+    <t>Method int lengthfloat(float[] mydata)</t>
+  </si>
+  <si>
+    <t>Method int lengthFloat(Float[] mydata)</t>
+  </si>
+  <si>
+    <t>Method int lengthFloatValue(FloatValue[] mydata)</t>
+  </si>
+  <si>
+    <t>Method int lengthdouble(double[] mydata)</t>
+  </si>
+  <si>
+    <t>Method int lengthDouble(Double[] mydata)</t>
+  </si>
+  <si>
+    <t>Method int lengthDoubleValue(DoubleValue[] mydata)</t>
+  </si>
+  <si>
+    <t>Method int lengthchar(char[] mydata)</t>
+  </si>
+  <si>
+    <t>Method int lengthCharacter(Character[] mydata)</t>
+  </si>
+  <si>
+    <t>Method int lengthboolean(boolean[] mydata)</t>
+  </si>
+  <si>
+    <t>Method int lengthBoolean(Boolean[] mydata)</t>
+  </si>
+  <si>
+    <t>Method int lengthBigInteger(BigInteger[] mydata)</t>
+  </si>
+  <si>
+    <t>Method int lengthBigIntegerValue(BigIntegerValue[] mydata)</t>
+  </si>
+  <si>
+    <t>Method int lengthBigDecimal(BigDecimal[] mydata)</t>
+  </si>
+  <si>
+    <t>Method int lengthBigDecimalValue(BigDecimalValue[] mydata)</t>
+  </si>
+  <si>
+    <t>Method int lengthString(String[] mydata)</t>
+  </si>
+  <si>
+    <t>Test lengthbyte</t>
+  </si>
+  <si>
+    <t>Test lengthByte</t>
+  </si>
+  <si>
+    <t>Test lengthByteValue</t>
+  </si>
+  <si>
+    <t>Test lengthshort</t>
+  </si>
+  <si>
+    <t>Test lengthShort</t>
+  </si>
+  <si>
+    <t>Test lengthShortValue</t>
+  </si>
+  <si>
+    <t>Test lengthint</t>
+  </si>
+  <si>
+    <t>Test lengthInteger</t>
+  </si>
+  <si>
+    <t>Test lengthIntValue</t>
+  </si>
+  <si>
+    <t>Test lengthlong</t>
+  </si>
+  <si>
+    <t>Test lengthLong</t>
+  </si>
+  <si>
+    <t>Test lengthLongValue</t>
+  </si>
+  <si>
+    <t>Test lengthfloat</t>
+  </si>
+  <si>
+    <t>Test lengthFloat</t>
+  </si>
+  <si>
+    <t>Test lengthFloatValue</t>
+  </si>
+  <si>
+    <t>Test lengthdouble</t>
+  </si>
+  <si>
+    <t>Test lengthDouble</t>
+  </si>
+  <si>
+    <t>Test lengthDoubleValue</t>
+  </si>
+  <si>
+    <t>Test lengthchar</t>
+  </si>
+  <si>
+    <t>Test lengthCharacter</t>
+  </si>
+  <si>
+    <t>Test lengthboolean</t>
+  </si>
+  <si>
+    <t>Test lengthBoolean</t>
+  </si>
+  <si>
+    <t>Test lengthBigInteger</t>
+  </si>
+  <si>
+    <t>Test lengthBigIntegerValue</t>
+  </si>
+  <si>
+    <t>Test lengthBigDecimal</t>
+  </si>
+  <si>
+    <t>Test lengthBigDecimalValue</t>
+  </si>
+  <si>
+    <t>Test lengthString</t>
+  </si>
+  <si>
+    <t>a,,,d</t>
+  </si>
+  <si>
+    <t>1,2,,,6</t>
+  </si>
+  <si>
+    <t>n,n,,,n</t>
+  </si>
+  <si>
+    <t>t,y,,,y</t>
+  </si>
+  <si>
+    <t>1,2,,,0</t>
   </si>
 </sst>
 </file>
@@ -2424,7 +2605,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -2474,6 +2655,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2782,7 +2965,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:K136"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H129" sqref="H129"/>
     </sheetView>
   </sheetViews>
@@ -2805,18 +2988,18 @@
       <c r="B3" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="40" t="s">
         <v>137</v>
       </c>
-      <c r="E3" s="38"/>
-      <c r="G3" s="38" t="s">
+      <c r="E3" s="40"/>
+      <c r="G3" s="40" t="s">
         <v>138</v>
       </c>
-      <c r="H3" s="38"/>
-      <c r="J3" s="38" t="s">
+      <c r="H3" s="40"/>
+      <c r="J3" s="40" t="s">
         <v>139</v>
       </c>
-      <c r="K3" s="38"/>
+      <c r="K3" s="40"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -2986,18 +3169,18 @@
       <c r="B16" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="D16" s="38" t="s">
+      <c r="D16" s="40" t="s">
         <v>140</v>
       </c>
-      <c r="E16" s="38"/>
-      <c r="G16" s="38" t="s">
+      <c r="E16" s="40"/>
+      <c r="G16" s="40" t="s">
         <v>141</v>
       </c>
-      <c r="H16" s="38"/>
-      <c r="J16" s="38" t="s">
+      <c r="H16" s="40"/>
+      <c r="J16" s="40" t="s">
         <v>142</v>
       </c>
-      <c r="K16" s="38"/>
+      <c r="K16" s="40"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
@@ -3169,18 +3352,18 @@
       <c r="B29" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="D29" s="38" t="s">
+      <c r="D29" s="40" t="s">
         <v>143</v>
       </c>
-      <c r="E29" s="38"/>
-      <c r="G29" s="38" t="s">
+      <c r="E29" s="40"/>
+      <c r="G29" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="H29" s="38"/>
-      <c r="J29" s="38" t="s">
+      <c r="H29" s="40"/>
+      <c r="J29" s="40" t="s">
         <v>145</v>
       </c>
-      <c r="K29" s="38"/>
+      <c r="K29" s="40"/>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
@@ -3364,18 +3547,18 @@
       <c r="B42" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="D42" s="38" t="s">
+      <c r="D42" s="40" t="s">
         <v>146</v>
       </c>
-      <c r="E42" s="38"/>
-      <c r="G42" s="38" t="s">
+      <c r="E42" s="40"/>
+      <c r="G42" s="40" t="s">
         <v>147</v>
       </c>
-      <c r="H42" s="38"/>
-      <c r="J42" s="38" t="s">
+      <c r="H42" s="40"/>
+      <c r="J42" s="40" t="s">
         <v>148</v>
       </c>
-      <c r="K42" s="38"/>
+      <c r="K42" s="40"/>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
@@ -3547,18 +3730,18 @@
       <c r="B55" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="D55" s="38" t="s">
+      <c r="D55" s="40" t="s">
         <v>149</v>
       </c>
-      <c r="E55" s="38"/>
-      <c r="G55" s="38" t="s">
+      <c r="E55" s="40"/>
+      <c r="G55" s="40" t="s">
         <v>150</v>
       </c>
-      <c r="H55" s="38"/>
-      <c r="J55" s="38" t="s">
+      <c r="H55" s="40"/>
+      <c r="J55" s="40" t="s">
         <v>151</v>
       </c>
-      <c r="K55" s="38"/>
+      <c r="K55" s="40"/>
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B56" s="2" t="s">
@@ -3724,18 +3907,18 @@
       <c r="B68" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="D68" s="38" t="s">
+      <c r="D68" s="40" t="s">
         <v>152</v>
       </c>
-      <c r="E68" s="38"/>
-      <c r="G68" s="38" t="s">
+      <c r="E68" s="40"/>
+      <c r="G68" s="40" t="s">
         <v>153</v>
       </c>
-      <c r="H68" s="38"/>
-      <c r="J68" s="38" t="s">
+      <c r="H68" s="40"/>
+      <c r="J68" s="40" t="s">
         <v>154</v>
       </c>
-      <c r="K68" s="38"/>
+      <c r="K68" s="40"/>
     </row>
     <row r="69" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B69" s="2" t="s">
@@ -3915,14 +4098,14 @@
       <c r="B81" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="D81" s="38" t="s">
+      <c r="D81" s="40" t="s">
         <v>155</v>
       </c>
-      <c r="E81" s="38"/>
-      <c r="G81" s="38" t="s">
+      <c r="E81" s="40"/>
+      <c r="G81" s="40" t="s">
         <v>156</v>
       </c>
-      <c r="H81" s="38"/>
+      <c r="H81" s="40"/>
     </row>
     <row r="82" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B82" s="2" t="s">
@@ -4052,14 +4235,14 @@
       <c r="B94" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="D94" s="38" t="s">
+      <c r="D94" s="40" t="s">
         <v>157</v>
       </c>
-      <c r="E94" s="38"/>
-      <c r="G94" s="38" t="s">
+      <c r="E94" s="40"/>
+      <c r="G94" s="40" t="s">
         <v>158</v>
       </c>
-      <c r="H94" s="38"/>
+      <c r="H94" s="40"/>
     </row>
     <row r="95" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B95" s="2" t="s">
@@ -4177,14 +4360,14 @@
       <c r="B105" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="D105" s="38" t="s">
+      <c r="D105" s="40" t="s">
         <v>159</v>
       </c>
-      <c r="E105" s="38"/>
-      <c r="G105" s="38" t="s">
+      <c r="E105" s="40"/>
+      <c r="G105" s="40" t="s">
         <v>160</v>
       </c>
-      <c r="H105" s="38"/>
+      <c r="H105" s="40"/>
     </row>
     <row r="106" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B106" s="2" t="s">
@@ -4297,14 +4480,14 @@
       <c r="B117" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="D117" s="38" t="s">
+      <c r="D117" s="40" t="s">
         <v>161</v>
       </c>
-      <c r="E117" s="38"/>
-      <c r="G117" s="38" t="s">
+      <c r="E117" s="40"/>
+      <c r="G117" s="40" t="s">
         <v>162</v>
       </c>
-      <c r="H117" s="38"/>
+      <c r="H117" s="40"/>
     </row>
     <row r="118" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B118" s="2" t="s">
@@ -4418,10 +4601,10 @@
         <v>198</v>
       </c>
       <c r="C130" s="12"/>
-      <c r="D130" s="39" t="s">
+      <c r="D130" s="41" t="s">
         <v>163</v>
       </c>
-      <c r="E130" s="39"/>
+      <c r="E130" s="41"/>
     </row>
     <row r="131" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B131" s="11" t="s">
@@ -4521,7 +4704,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:K136"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -4544,18 +4727,18 @@
       <c r="B3" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="40" t="s">
         <v>200</v>
       </c>
-      <c r="E3" s="38"/>
-      <c r="G3" s="38" t="s">
+      <c r="E3" s="40"/>
+      <c r="G3" s="40" t="s">
         <v>201</v>
       </c>
-      <c r="H3" s="38"/>
-      <c r="J3" s="38" t="s">
+      <c r="H3" s="40"/>
+      <c r="J3" s="40" t="s">
         <v>202</v>
       </c>
-      <c r="K3" s="38"/>
+      <c r="K3" s="40"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -4725,18 +4908,18 @@
       <c r="B16" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="D16" s="38" t="s">
+      <c r="D16" s="40" t="s">
         <v>207</v>
       </c>
-      <c r="E16" s="38"/>
-      <c r="G16" s="38" t="s">
+      <c r="E16" s="40"/>
+      <c r="G16" s="40" t="s">
         <v>208</v>
       </c>
-      <c r="H16" s="38"/>
-      <c r="J16" s="38" t="s">
+      <c r="H16" s="40"/>
+      <c r="J16" s="40" t="s">
         <v>209</v>
       </c>
-      <c r="K16" s="38"/>
+      <c r="K16" s="40"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
@@ -4908,18 +5091,18 @@
       <c r="B29" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="D29" s="38" t="s">
+      <c r="D29" s="40" t="s">
         <v>213</v>
       </c>
-      <c r="E29" s="38"/>
-      <c r="G29" s="38" t="s">
+      <c r="E29" s="40"/>
+      <c r="G29" s="40" t="s">
         <v>214</v>
       </c>
-      <c r="H29" s="38"/>
-      <c r="J29" s="38" t="s">
+      <c r="H29" s="40"/>
+      <c r="J29" s="40" t="s">
         <v>215</v>
       </c>
-      <c r="K29" s="38"/>
+      <c r="K29" s="40"/>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
@@ -5103,18 +5286,18 @@
       <c r="B42" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="D42" s="38" t="s">
+      <c r="D42" s="40" t="s">
         <v>219</v>
       </c>
-      <c r="E42" s="38"/>
-      <c r="G42" s="38" t="s">
+      <c r="E42" s="40"/>
+      <c r="G42" s="40" t="s">
         <v>220</v>
       </c>
-      <c r="H42" s="38"/>
-      <c r="J42" s="38" t="s">
+      <c r="H42" s="40"/>
+      <c r="J42" s="40" t="s">
         <v>221</v>
       </c>
-      <c r="K42" s="38"/>
+      <c r="K42" s="40"/>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
@@ -5286,18 +5469,18 @@
       <c r="B55" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="D55" s="38" t="s">
+      <c r="D55" s="40" t="s">
         <v>225</v>
       </c>
-      <c r="E55" s="38"/>
-      <c r="G55" s="38" t="s">
+      <c r="E55" s="40"/>
+      <c r="G55" s="40" t="s">
         <v>226</v>
       </c>
-      <c r="H55" s="38"/>
-      <c r="J55" s="38" t="s">
+      <c r="H55" s="40"/>
+      <c r="J55" s="40" t="s">
         <v>227</v>
       </c>
-      <c r="K55" s="38"/>
+      <c r="K55" s="40"/>
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B56" s="2" t="s">
@@ -5463,18 +5646,18 @@
       <c r="B68" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="D68" s="38" t="s">
+      <c r="D68" s="40" t="s">
         <v>231</v>
       </c>
-      <c r="E68" s="38"/>
-      <c r="G68" s="38" t="s">
+      <c r="E68" s="40"/>
+      <c r="G68" s="40" t="s">
         <v>232</v>
       </c>
-      <c r="H68" s="38"/>
-      <c r="J68" s="38" t="s">
+      <c r="H68" s="40"/>
+      <c r="J68" s="40" t="s">
         <v>233</v>
       </c>
-      <c r="K68" s="38"/>
+      <c r="K68" s="40"/>
     </row>
     <row r="69" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B69" s="2" t="s">
@@ -5654,14 +5837,14 @@
       <c r="B81" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="D81" s="38" t="s">
+      <c r="D81" s="40" t="s">
         <v>237</v>
       </c>
-      <c r="E81" s="38"/>
-      <c r="G81" s="38" t="s">
+      <c r="E81" s="40"/>
+      <c r="G81" s="40" t="s">
         <v>238</v>
       </c>
-      <c r="H81" s="38"/>
+      <c r="H81" s="40"/>
     </row>
     <row r="82" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B82" s="2" t="s">
@@ -5791,14 +5974,14 @@
       <c r="B94" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="D94" s="38" t="s">
+      <c r="D94" s="40" t="s">
         <v>241</v>
       </c>
-      <c r="E94" s="38"/>
-      <c r="G94" s="38" t="s">
+      <c r="E94" s="40"/>
+      <c r="G94" s="40" t="s">
         <v>242</v>
       </c>
-      <c r="H94" s="38"/>
+      <c r="H94" s="40"/>
     </row>
     <row r="95" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B95" s="2" t="s">
@@ -5916,14 +6099,14 @@
       <c r="B105" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="D105" s="38" t="s">
+      <c r="D105" s="40" t="s">
         <v>245</v>
       </c>
-      <c r="E105" s="38"/>
-      <c r="G105" s="38" t="s">
+      <c r="E105" s="40"/>
+      <c r="G105" s="40" t="s">
         <v>246</v>
       </c>
-      <c r="H105" s="38"/>
+      <c r="H105" s="40"/>
     </row>
     <row r="106" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B106" s="2" t="s">
@@ -6036,14 +6219,14 @@
       <c r="B117" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="D117" s="38" t="s">
+      <c r="D117" s="40" t="s">
         <v>249</v>
       </c>
-      <c r="E117" s="38"/>
-      <c r="G117" s="38" t="s">
+      <c r="E117" s="40"/>
+      <c r="G117" s="40" t="s">
         <v>250</v>
       </c>
-      <c r="H117" s="38"/>
+      <c r="H117" s="40"/>
     </row>
     <row r="118" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B118" s="2" t="s">
@@ -6157,10 +6340,10 @@
         <v>252</v>
       </c>
       <c r="C130" s="12"/>
-      <c r="D130" s="39" t="s">
+      <c r="D130" s="41" t="s">
         <v>253</v>
       </c>
-      <c r="E130" s="39"/>
+      <c r="E130" s="41"/>
     </row>
     <row r="131" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B131" s="11" t="s">
@@ -6285,21 +6468,21 @@
       <c r="B3" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="40" t="s">
         <v>254</v>
       </c>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="H3" s="38" t="s">
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="H3" s="40" t="s">
         <v>255</v>
       </c>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="L3" s="38" t="s">
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="L3" s="40" t="s">
         <v>256</v>
       </c>
-      <c r="M3" s="38"/>
-      <c r="N3" s="38"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="40"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -6568,21 +6751,21 @@
       <c r="B16" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="D16" s="38" t="s">
+      <c r="D16" s="40" t="s">
         <v>257</v>
       </c>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="H16" s="38" t="s">
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="H16" s="40" t="s">
         <v>258</v>
       </c>
-      <c r="I16" s="38"/>
-      <c r="J16" s="38"/>
-      <c r="L16" s="38" t="s">
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
+      <c r="L16" s="40" t="s">
         <v>259</v>
       </c>
-      <c r="M16" s="38"/>
-      <c r="N16" s="38"/>
+      <c r="M16" s="40"/>
+      <c r="N16" s="40"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
@@ -6850,21 +7033,21 @@
       <c r="B29" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="D29" s="38" t="s">
+      <c r="D29" s="40" t="s">
         <v>260</v>
       </c>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="H29" s="38" t="s">
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="H29" s="40" t="s">
         <v>261</v>
       </c>
-      <c r="I29" s="38"/>
-      <c r="J29" s="38"/>
-      <c r="L29" s="38" t="s">
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
+      <c r="L29" s="40" t="s">
         <v>262</v>
       </c>
-      <c r="M29" s="38"/>
-      <c r="N29" s="38"/>
+      <c r="M29" s="40"/>
+      <c r="N29" s="40"/>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
@@ -7153,21 +7336,21 @@
       <c r="B42" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="D42" s="38" t="s">
+      <c r="D42" s="40" t="s">
         <v>263</v>
       </c>
-      <c r="E42" s="38"/>
-      <c r="F42" s="38"/>
-      <c r="H42" s="38" t="s">
+      <c r="E42" s="40"/>
+      <c r="F42" s="40"/>
+      <c r="H42" s="40" t="s">
         <v>264</v>
       </c>
-      <c r="I42" s="38"/>
-      <c r="J42" s="38"/>
-      <c r="L42" s="38" t="s">
+      <c r="I42" s="40"/>
+      <c r="J42" s="40"/>
+      <c r="L42" s="40" t="s">
         <v>265</v>
       </c>
-      <c r="M42" s="38"/>
-      <c r="N42" s="38"/>
+      <c r="M42" s="40"/>
+      <c r="N42" s="40"/>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
@@ -7435,21 +7618,21 @@
       <c r="B55" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="D55" s="38" t="s">
+      <c r="D55" s="40" t="s">
         <v>266</v>
       </c>
-      <c r="E55" s="38"/>
-      <c r="F55" s="38"/>
-      <c r="H55" s="38" t="s">
+      <c r="E55" s="40"/>
+      <c r="F55" s="40"/>
+      <c r="H55" s="40" t="s">
         <v>267</v>
       </c>
-      <c r="I55" s="38"/>
-      <c r="J55" s="38"/>
-      <c r="L55" s="38" t="s">
+      <c r="I55" s="40"/>
+      <c r="J55" s="40"/>
+      <c r="L55" s="40" t="s">
         <v>268</v>
       </c>
-      <c r="M55" s="38"/>
-      <c r="N55" s="38"/>
+      <c r="M55" s="40"/>
+      <c r="N55" s="40"/>
     </row>
     <row r="56" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B56" s="2" t="s">
@@ -7711,21 +7894,21 @@
       <c r="B68" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="D68" s="38" t="s">
+      <c r="D68" s="40" t="s">
         <v>269</v>
       </c>
-      <c r="E68" s="38"/>
-      <c r="F68" s="38"/>
-      <c r="H68" s="38" t="s">
+      <c r="E68" s="40"/>
+      <c r="F68" s="40"/>
+      <c r="H68" s="40" t="s">
         <v>270</v>
       </c>
-      <c r="I68" s="38"/>
-      <c r="J68" s="38"/>
-      <c r="L68" s="38" t="s">
+      <c r="I68" s="40"/>
+      <c r="J68" s="40"/>
+      <c r="L68" s="40" t="s">
         <v>271</v>
       </c>
-      <c r="M68" s="38"/>
-      <c r="N68" s="38"/>
+      <c r="M68" s="40"/>
+      <c r="N68" s="40"/>
     </row>
     <row r="69" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B69" s="2" t="s">
@@ -8006,16 +8189,16 @@
       <c r="B81" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="D81" s="38" t="s">
+      <c r="D81" s="40" t="s">
         <v>272</v>
       </c>
-      <c r="E81" s="38"/>
-      <c r="F81" s="38"/>
-      <c r="H81" s="38" t="s">
+      <c r="E81" s="40"/>
+      <c r="F81" s="40"/>
+      <c r="H81" s="40" t="s">
         <v>273</v>
       </c>
-      <c r="I81" s="38"/>
-      <c r="J81" s="38"/>
+      <c r="I81" s="40"/>
+      <c r="J81" s="40"/>
     </row>
     <row r="82" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B82" s="2" t="s">
@@ -8207,16 +8390,16 @@
       <c r="B94" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="D94" s="38" t="s">
+      <c r="D94" s="40" t="s">
         <v>274</v>
       </c>
-      <c r="E94" s="38"/>
-      <c r="F94" s="38"/>
-      <c r="H94" s="38" t="s">
+      <c r="E94" s="40"/>
+      <c r="F94" s="40"/>
+      <c r="H94" s="40" t="s">
         <v>275</v>
       </c>
-      <c r="I94" s="38"/>
-      <c r="J94" s="38"/>
+      <c r="I94" s="40"/>
+      <c r="J94" s="40"/>
     </row>
     <row r="95" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B95" s="2" t="s">
@@ -8404,16 +8587,16 @@
       <c r="B107" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="D107" s="38" t="s">
+      <c r="D107" s="40" t="s">
         <v>276</v>
       </c>
-      <c r="E107" s="38"/>
-      <c r="F107" s="38"/>
-      <c r="H107" s="38" t="s">
+      <c r="E107" s="40"/>
+      <c r="F107" s="40"/>
+      <c r="H107" s="40" t="s">
         <v>277</v>
       </c>
-      <c r="I107" s="38"/>
-      <c r="J107" s="38"/>
+      <c r="I107" s="40"/>
+      <c r="J107" s="40"/>
     </row>
     <row r="108" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B108" s="2" t="s">
@@ -8604,16 +8787,16 @@
       <c r="B120" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="D120" s="38" t="s">
+      <c r="D120" s="40" t="s">
         <v>278</v>
       </c>
-      <c r="E120" s="38"/>
-      <c r="F120" s="38"/>
-      <c r="H120" s="38" t="s">
+      <c r="E120" s="40"/>
+      <c r="F120" s="40"/>
+      <c r="H120" s="40" t="s">
         <v>279</v>
       </c>
-      <c r="I120" s="38"/>
-      <c r="J120" s="38"/>
+      <c r="I120" s="40"/>
+      <c r="J120" s="40"/>
     </row>
     <row r="121" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B121" s="2" t="s">
@@ -8802,11 +8985,11 @@
         <v>318</v>
       </c>
       <c r="C133" s="12"/>
-      <c r="D133" s="39" t="s">
+      <c r="D133" s="41" t="s">
         <v>280</v>
       </c>
-      <c r="E133" s="39"/>
-      <c r="F133" s="39"/>
+      <c r="E133" s="41"/>
+      <c r="F133" s="41"/>
     </row>
     <row r="134" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B134" s="2" t="s">
@@ -8954,7 +9137,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:Q142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B73" workbookViewId="0">
+    <sheetView topLeftCell="B73" workbookViewId="0">
       <selection activeCell="I104" sqref="I104"/>
     </sheetView>
   </sheetViews>
@@ -8981,24 +9164,24 @@
       <c r="B3" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="40" t="s">
         <v>324</v>
       </c>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="I3" s="38" t="s">
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="I3" s="40" t="s">
         <v>325</v>
       </c>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="N3" s="38" t="s">
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="N3" s="40" t="s">
         <v>326</v>
       </c>
-      <c r="O3" s="38"/>
-      <c r="P3" s="38"/>
-      <c r="Q3" s="38"/>
+      <c r="O3" s="40"/>
+      <c r="P3" s="40"/>
+      <c r="Q3" s="40"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -9346,24 +9529,24 @@
       <c r="B16" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="D16" s="38" t="s">
+      <c r="D16" s="40" t="s">
         <v>327</v>
       </c>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="I16" s="38" t="s">
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="I16" s="40" t="s">
         <v>328</v>
       </c>
-      <c r="J16" s="38"/>
-      <c r="K16" s="38"/>
-      <c r="L16" s="38"/>
-      <c r="N16" s="38" t="s">
+      <c r="J16" s="40"/>
+      <c r="K16" s="40"/>
+      <c r="L16" s="40"/>
+      <c r="N16" s="40" t="s">
         <v>329</v>
       </c>
-      <c r="O16" s="38"/>
-      <c r="P16" s="38"/>
-      <c r="Q16" s="38"/>
+      <c r="O16" s="40"/>
+      <c r="P16" s="40"/>
+      <c r="Q16" s="40"/>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
@@ -9709,24 +9892,24 @@
       <c r="B29" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="D29" s="38" t="s">
+      <c r="D29" s="40" t="s">
         <v>330</v>
       </c>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="38"/>
-      <c r="I29" s="38" t="s">
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="I29" s="40" t="s">
         <v>331</v>
       </c>
-      <c r="J29" s="38"/>
-      <c r="K29" s="38"/>
-      <c r="L29" s="38"/>
-      <c r="N29" s="38" t="s">
+      <c r="J29" s="40"/>
+      <c r="K29" s="40"/>
+      <c r="L29" s="40"/>
+      <c r="N29" s="40" t="s">
         <v>332</v>
       </c>
-      <c r="O29" s="38"/>
-      <c r="P29" s="38"/>
-      <c r="Q29" s="38"/>
+      <c r="O29" s="40"/>
+      <c r="P29" s="40"/>
+      <c r="Q29" s="40"/>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
@@ -10100,24 +10283,24 @@
       <c r="B42" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="D42" s="38" t="s">
+      <c r="D42" s="40" t="s">
         <v>333</v>
       </c>
-      <c r="E42" s="38"/>
-      <c r="F42" s="38"/>
-      <c r="G42" s="38"/>
-      <c r="I42" s="38" t="s">
+      <c r="E42" s="40"/>
+      <c r="F42" s="40"/>
+      <c r="G42" s="40"/>
+      <c r="I42" s="40" t="s">
         <v>334</v>
       </c>
-      <c r="J42" s="38"/>
-      <c r="K42" s="38"/>
-      <c r="L42" s="38"/>
-      <c r="N42" s="38" t="s">
+      <c r="J42" s="40"/>
+      <c r="K42" s="40"/>
+      <c r="L42" s="40"/>
+      <c r="N42" s="40" t="s">
         <v>335</v>
       </c>
-      <c r="O42" s="38"/>
-      <c r="P42" s="38"/>
-      <c r="Q42" s="38"/>
+      <c r="O42" s="40"/>
+      <c r="P42" s="40"/>
+      <c r="Q42" s="40"/>
     </row>
     <row r="43" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
@@ -10463,24 +10646,24 @@
       <c r="B55" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="D55" s="38" t="s">
+      <c r="D55" s="40" t="s">
         <v>336</v>
       </c>
-      <c r="E55" s="38"/>
-      <c r="F55" s="38"/>
-      <c r="G55" s="38"/>
-      <c r="I55" s="38" t="s">
+      <c r="E55" s="40"/>
+      <c r="F55" s="40"/>
+      <c r="G55" s="40"/>
+      <c r="I55" s="40" t="s">
         <v>337</v>
       </c>
-      <c r="J55" s="38"/>
-      <c r="K55" s="38"/>
-      <c r="L55" s="38"/>
-      <c r="N55" s="38" t="s">
+      <c r="J55" s="40"/>
+      <c r="K55" s="40"/>
+      <c r="L55" s="40"/>
+      <c r="N55" s="40" t="s">
         <v>338</v>
       </c>
-      <c r="O55" s="38"/>
-      <c r="P55" s="38"/>
-      <c r="Q55" s="38"/>
+      <c r="O55" s="40"/>
+      <c r="P55" s="40"/>
+      <c r="Q55" s="40"/>
     </row>
     <row r="56" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B56" s="2" t="s">
@@ -10820,24 +11003,24 @@
       <c r="B68" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="D68" s="38" t="s">
+      <c r="D68" s="40" t="s">
         <v>339</v>
       </c>
-      <c r="E68" s="38"/>
-      <c r="F68" s="38"/>
-      <c r="G68" s="38"/>
-      <c r="I68" s="38" t="s">
+      <c r="E68" s="40"/>
+      <c r="F68" s="40"/>
+      <c r="G68" s="40"/>
+      <c r="I68" s="40" t="s">
         <v>340</v>
       </c>
-      <c r="J68" s="38"/>
-      <c r="K68" s="38"/>
-      <c r="L68" s="38"/>
-      <c r="N68" s="38" t="s">
+      <c r="J68" s="40"/>
+      <c r="K68" s="40"/>
+      <c r="L68" s="40"/>
+      <c r="N68" s="40" t="s">
         <v>341</v>
       </c>
-      <c r="O68" s="38"/>
-      <c r="P68" s="38"/>
-      <c r="Q68" s="38"/>
+      <c r="O68" s="40"/>
+      <c r="P68" s="40"/>
+      <c r="Q68" s="40"/>
     </row>
     <row r="69" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B69" s="2" t="s">
@@ -11200,18 +11383,18 @@
       <c r="B81" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="D81" s="38" t="s">
+      <c r="D81" s="40" t="s">
         <v>342</v>
       </c>
-      <c r="E81" s="38"/>
-      <c r="F81" s="38"/>
-      <c r="G81" s="38"/>
-      <c r="I81" s="38" t="s">
+      <c r="E81" s="40"/>
+      <c r="F81" s="40"/>
+      <c r="G81" s="40"/>
+      <c r="I81" s="40" t="s">
         <v>343</v>
       </c>
-      <c r="J81" s="38"/>
-      <c r="K81" s="38"/>
-      <c r="L81" s="38"/>
+      <c r="J81" s="40"/>
+      <c r="K81" s="40"/>
+      <c r="L81" s="40"/>
     </row>
     <row r="82" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B82" s="2" t="s">
@@ -11454,18 +11637,18 @@
       <c r="B94" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="D94" s="38" t="s">
+      <c r="D94" s="40" t="s">
         <v>344</v>
       </c>
-      <c r="E94" s="38"/>
-      <c r="F94" s="38"/>
-      <c r="G94" s="38"/>
-      <c r="I94" s="38" t="s">
+      <c r="E94" s="40"/>
+      <c r="F94" s="40"/>
+      <c r="G94" s="40"/>
+      <c r="I94" s="40" t="s">
         <v>345</v>
       </c>
-      <c r="J94" s="38"/>
-      <c r="K94" s="38"/>
-      <c r="L94" s="38"/>
+      <c r="J94" s="40"/>
+      <c r="K94" s="40"/>
+      <c r="L94" s="40"/>
     </row>
     <row r="95" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B95" s="2" t="s">
@@ -11706,18 +11889,18 @@
       <c r="B107" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="D107" s="38" t="s">
+      <c r="D107" s="40" t="s">
         <v>346</v>
       </c>
-      <c r="E107" s="38"/>
-      <c r="F107" s="38"/>
-      <c r="G107" s="38"/>
-      <c r="I107" s="38" t="s">
+      <c r="E107" s="40"/>
+      <c r="F107" s="40"/>
+      <c r="G107" s="40"/>
+      <c r="I107" s="40" t="s">
         <v>347</v>
       </c>
-      <c r="J107" s="38"/>
-      <c r="K107" s="38"/>
-      <c r="L107" s="38"/>
+      <c r="J107" s="40"/>
+      <c r="K107" s="40"/>
+      <c r="L107" s="40"/>
     </row>
     <row r="108" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B108" s="2" t="s">
@@ -11964,18 +12147,18 @@
       <c r="B120" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="D120" s="38" t="s">
+      <c r="D120" s="40" t="s">
         <v>348</v>
       </c>
-      <c r="E120" s="38"/>
-      <c r="F120" s="38"/>
-      <c r="G120" s="38"/>
-      <c r="I120" s="38" t="s">
+      <c r="E120" s="40"/>
+      <c r="F120" s="40"/>
+      <c r="G120" s="40"/>
+      <c r="I120" s="40" t="s">
         <v>349</v>
       </c>
-      <c r="J120" s="38"/>
-      <c r="K120" s="38"/>
-      <c r="L120" s="38"/>
+      <c r="J120" s="40"/>
+      <c r="K120" s="40"/>
+      <c r="L120" s="40"/>
     </row>
     <row r="121" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B121" s="2" t="s">
@@ -12219,12 +12402,12 @@
         <v>377</v>
       </c>
       <c r="C133" s="12"/>
-      <c r="D133" s="39" t="s">
+      <c r="D133" s="41" t="s">
         <v>350</v>
       </c>
-      <c r="E133" s="39"/>
-      <c r="F133" s="39"/>
-      <c r="G133" s="39"/>
+      <c r="E133" s="41"/>
+      <c r="F133" s="41"/>
+      <c r="G133" s="41"/>
     </row>
     <row r="134" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B134" s="2" t="s">
@@ -12421,21 +12604,21 @@
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="H3" s="38" t="s">
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="H3" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="L3" s="38" t="s">
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="L3" s="40" t="s">
         <v>124</v>
       </c>
-      <c r="M3" s="38"/>
-      <c r="N3" s="38"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="40"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -12704,21 +12887,21 @@
         <v>1</v>
       </c>
       <c r="C16" s="3"/>
-      <c r="D16" s="38" t="s">
+      <c r="D16" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="H16" s="38" t="s">
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="H16" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="I16" s="38"/>
-      <c r="J16" s="38"/>
-      <c r="L16" s="38" t="s">
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
+      <c r="L16" s="40" t="s">
         <v>125</v>
       </c>
-      <c r="M16" s="38"/>
-      <c r="N16" s="38"/>
+      <c r="M16" s="40"/>
+      <c r="N16" s="40"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
@@ -12979,21 +13162,21 @@
       <c r="B29" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D29" s="38" t="s">
+      <c r="D29" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="H29" s="38" t="s">
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="H29" s="40" t="s">
         <v>120</v>
       </c>
-      <c r="I29" s="38"/>
-      <c r="J29" s="38"/>
-      <c r="L29" s="38" t="s">
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
+      <c r="L29" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="M29" s="38"/>
-      <c r="N29" s="38"/>
+      <c r="M29" s="40"/>
+      <c r="N29" s="40"/>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
@@ -13280,21 +13463,21 @@
       <c r="B42" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D42" s="38" t="s">
+      <c r="D42" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="E42" s="38"/>
-      <c r="F42" s="38"/>
-      <c r="H42" s="38" t="s">
+      <c r="E42" s="40"/>
+      <c r="F42" s="40"/>
+      <c r="H42" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="I42" s="38"/>
-      <c r="J42" s="38"/>
-      <c r="L42" s="38" t="s">
+      <c r="I42" s="40"/>
+      <c r="J42" s="40"/>
+      <c r="L42" s="40" t="s">
         <v>129</v>
       </c>
-      <c r="M42" s="38"/>
-      <c r="N42" s="38"/>
+      <c r="M42" s="40"/>
+      <c r="N42" s="40"/>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
@@ -13554,21 +13737,21 @@
       <c r="B55" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D55" s="38" t="s">
+      <c r="D55" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="E55" s="38"/>
-      <c r="F55" s="38"/>
-      <c r="H55" s="38" t="s">
+      <c r="E55" s="40"/>
+      <c r="F55" s="40"/>
+      <c r="H55" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="I55" s="38"/>
-      <c r="J55" s="38"/>
-      <c r="L55" s="38" t="s">
+      <c r="I55" s="40"/>
+      <c r="J55" s="40"/>
+      <c r="L55" s="40" t="s">
         <v>130</v>
       </c>
-      <c r="M55" s="38"/>
-      <c r="N55" s="38"/>
+      <c r="M55" s="40"/>
+      <c r="N55" s="40"/>
     </row>
     <row r="56" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B56" s="2" t="s">
@@ -13864,21 +14047,21 @@
       <c r="B69" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D69" s="38" t="s">
+      <c r="D69" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="E69" s="38"/>
-      <c r="F69" s="38"/>
-      <c r="H69" s="38" t="s">
+      <c r="E69" s="40"/>
+      <c r="F69" s="40"/>
+      <c r="H69" s="40" t="s">
         <v>87</v>
       </c>
-      <c r="I69" s="38"/>
-      <c r="J69" s="38"/>
-      <c r="L69" s="38" t="s">
+      <c r="I69" s="40"/>
+      <c r="J69" s="40"/>
+      <c r="L69" s="40" t="s">
         <v>131</v>
       </c>
-      <c r="M69" s="38"/>
-      <c r="N69" s="38"/>
+      <c r="M69" s="40"/>
+      <c r="N69" s="40"/>
     </row>
     <row r="70" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B70" s="2" t="s">
@@ -14184,16 +14367,16 @@
       <c r="B83" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D83" s="38" t="s">
+      <c r="D83" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="E83" s="38"/>
-      <c r="F83" s="38"/>
-      <c r="H83" s="38" t="s">
+      <c r="E83" s="40"/>
+      <c r="F83" s="40"/>
+      <c r="H83" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="I83" s="38"/>
-      <c r="J83" s="38"/>
+      <c r="I83" s="40"/>
+      <c r="J83" s="40"/>
     </row>
     <row r="84" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B84" s="2" t="s">
@@ -14405,16 +14588,16 @@
       <c r="B96" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D96" s="38" t="s">
+      <c r="D96" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="E96" s="38"/>
-      <c r="F96" s="38"/>
-      <c r="H96" s="38" t="s">
+      <c r="E96" s="40"/>
+      <c r="F96" s="40"/>
+      <c r="H96" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="I96" s="38"/>
-      <c r="J96" s="38"/>
+      <c r="I96" s="40"/>
+      <c r="J96" s="40"/>
     </row>
     <row r="97" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B97" s="2" t="s">
@@ -14585,16 +14768,16 @@
         <v>31</v>
       </c>
       <c r="C107" s="3"/>
-      <c r="D107" s="38" t="s">
+      <c r="D107" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="E107" s="38"/>
-      <c r="F107" s="38"/>
-      <c r="H107" s="38" t="s">
+      <c r="E107" s="40"/>
+      <c r="F107" s="40"/>
+      <c r="H107" s="40" t="s">
         <v>133</v>
       </c>
-      <c r="I107" s="38"/>
-      <c r="J107" s="38"/>
+      <c r="I107" s="40"/>
+      <c r="J107" s="40"/>
     </row>
     <row r="108" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B108" s="2" t="s">
@@ -14796,16 +14979,16 @@
         <v>32</v>
       </c>
       <c r="C119" s="3"/>
-      <c r="D119" s="38" t="s">
+      <c r="D119" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="E119" s="38"/>
-      <c r="F119" s="38"/>
-      <c r="H119" s="38" t="s">
+      <c r="E119" s="40"/>
+      <c r="F119" s="40"/>
+      <c r="H119" s="40" t="s">
         <v>135</v>
       </c>
-      <c r="I119" s="38"/>
-      <c r="J119" s="38"/>
+      <c r="I119" s="40"/>
+      <c r="J119" s="40"/>
     </row>
     <row r="120" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B120" s="2" t="s">
@@ -15019,11 +15202,11 @@
         <v>41</v>
       </c>
       <c r="C132" s="12"/>
-      <c r="D132" s="39" t="s">
+      <c r="D132" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="E132" s="39"/>
-      <c r="F132" s="39"/>
+      <c r="E132" s="41"/>
+      <c r="F132" s="41"/>
     </row>
     <row r="133" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B133" s="11" t="s">
@@ -15178,7 +15361,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="F3:P152"/>
   <sheetViews>
-    <sheetView topLeftCell="A91" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F132" sqref="F132"/>
     </sheetView>
   </sheetViews>
@@ -15201,16 +15384,16 @@
       <c r="F3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="38" t="s">
+      <c r="J3" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="N3" s="38" t="s">
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="N3" s="40" t="s">
         <v>99</v>
       </c>
-      <c r="O3" s="38"/>
-      <c r="P3" s="38"/>
+      <c r="O3" s="40"/>
+      <c r="P3" s="40"/>
     </row>
     <row r="4" spans="6:16" x14ac:dyDescent="0.25">
       <c r="F4" s="2" t="s">
@@ -15379,16 +15562,16 @@
       <c r="F16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J16" s="38" t="s">
+      <c r="J16" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="K16" s="38"/>
-      <c r="L16" s="38"/>
-      <c r="N16" s="38" t="s">
+      <c r="K16" s="40"/>
+      <c r="L16" s="40"/>
+      <c r="N16" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="O16" s="38"/>
-      <c r="P16" s="38"/>
+      <c r="O16" s="40"/>
+      <c r="P16" s="40"/>
     </row>
     <row r="17" spans="6:16" x14ac:dyDescent="0.25">
       <c r="F17" s="2" t="s">
@@ -15553,11 +15736,11 @@
       <c r="F29" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J29" s="38" t="s">
+      <c r="J29" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="K29" s="38"/>
-      <c r="L29" s="38"/>
+      <c r="K29" s="40"/>
+      <c r="L29" s="40"/>
     </row>
     <row r="30" spans="6:16" x14ac:dyDescent="0.25">
       <c r="F30" s="2" t="s">
@@ -15644,16 +15827,16 @@
       <c r="F40" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J40" s="38" t="s">
+      <c r="J40" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="K40" s="38"/>
-      <c r="L40" s="38"/>
-      <c r="N40" s="38" t="s">
+      <c r="K40" s="40"/>
+      <c r="L40" s="40"/>
+      <c r="N40" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="O40" s="38"/>
-      <c r="P40" s="38"/>
+      <c r="O40" s="40"/>
+      <c r="P40" s="40"/>
     </row>
     <row r="41" spans="6:16" x14ac:dyDescent="0.25">
       <c r="F41" s="2" t="s">
@@ -15818,16 +16001,16 @@
       <c r="F53" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J53" s="38" t="s">
+      <c r="J53" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="K53" s="38"/>
-      <c r="L53" s="38"/>
-      <c r="N53" s="38" t="s">
+      <c r="K53" s="40"/>
+      <c r="L53" s="40"/>
+      <c r="N53" s="40" t="s">
         <v>110</v>
       </c>
-      <c r="O53" s="38"/>
-      <c r="P53" s="38"/>
+      <c r="O53" s="40"/>
+      <c r="P53" s="40"/>
     </row>
     <row r="54" spans="6:16" x14ac:dyDescent="0.25">
       <c r="F54" s="2" t="s">
@@ -16012,16 +16195,16 @@
       <c r="F67" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J67" s="38" t="s">
+      <c r="J67" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="K67" s="38"/>
-      <c r="L67" s="38"/>
-      <c r="N67" s="38" t="s">
+      <c r="K67" s="40"/>
+      <c r="L67" s="40"/>
+      <c r="N67" s="40" t="s">
         <v>112</v>
       </c>
-      <c r="O67" s="38"/>
-      <c r="P67" s="38"/>
+      <c r="O67" s="40"/>
+      <c r="P67" s="40"/>
     </row>
     <row r="68" spans="6:16" x14ac:dyDescent="0.25">
       <c r="F68" s="2" t="s">
@@ -16206,16 +16389,16 @@
       <c r="F81" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J81" s="38" t="s">
+      <c r="J81" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="K81" s="38"/>
-      <c r="L81" s="38"/>
-      <c r="N81" s="38" t="s">
+      <c r="K81" s="40"/>
+      <c r="L81" s="40"/>
+      <c r="N81" s="40" t="s">
         <v>113</v>
       </c>
-      <c r="O81" s="38"/>
-      <c r="P81" s="38"/>
+      <c r="O81" s="40"/>
+      <c r="P81" s="40"/>
     </row>
     <row r="82" spans="6:16" x14ac:dyDescent="0.25">
       <c r="F82" s="2" t="s">
@@ -16384,16 +16567,16 @@
       <c r="F94" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J94" s="38" t="s">
+      <c r="J94" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="K94" s="38"/>
-      <c r="L94" s="38"/>
-      <c r="N94" s="38" t="s">
+      <c r="K94" s="40"/>
+      <c r="L94" s="40"/>
+      <c r="N94" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="O94" s="38"/>
-      <c r="P94" s="38"/>
+      <c r="O94" s="40"/>
+      <c r="P94" s="40"/>
     </row>
     <row r="95" spans="6:16" x14ac:dyDescent="0.25">
       <c r="F95" s="2" t="s">
@@ -16546,11 +16729,11 @@
       <c r="G104" s="12"/>
       <c r="H104" s="12"/>
       <c r="I104" s="12"/>
-      <c r="J104" s="39" t="s">
+      <c r="J104" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="K104" s="39"/>
-      <c r="L104" s="39"/>
+      <c r="K104" s="41"/>
+      <c r="L104" s="41"/>
     </row>
     <row r="105" spans="6:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F105" s="11" t="s">
@@ -16714,11 +16897,11 @@
       <c r="G117" s="12"/>
       <c r="H117" s="12"/>
       <c r="I117" s="12"/>
-      <c r="J117" s="39" t="s">
+      <c r="J117" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="K117" s="39"/>
-      <c r="L117" s="39"/>
+      <c r="K117" s="41"/>
+      <c r="L117" s="41"/>
     </row>
     <row r="118" spans="6:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F118" s="11" t="s">
@@ -16897,11 +17080,11 @@
       <c r="G131" s="12"/>
       <c r="H131" s="12"/>
       <c r="I131" s="12"/>
-      <c r="J131" s="39" t="s">
+      <c r="J131" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="K131" s="39"/>
-      <c r="L131" s="39"/>
+      <c r="K131" s="41"/>
+      <c r="L131" s="41"/>
     </row>
     <row r="132" spans="6:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F132" s="11" t="s">
@@ -17037,11 +17220,11 @@
       <c r="F144" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="J144" s="38" t="s">
+      <c r="J144" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="K144" s="38"/>
-      <c r="L144" s="38"/>
+      <c r="K144" s="40"/>
+      <c r="L144" s="40"/>
     </row>
     <row r="145" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F145" s="2" t="s">
@@ -17190,11 +17373,11 @@
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
       <c r="I3" s="12"/>
-      <c r="J3" s="39" t="s">
+      <c r="J3" s="41" t="s">
         <v>94</v>
       </c>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
     </row>
     <row r="4" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F4" s="11" t="s">
@@ -17312,4 +17495,1741 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:K136"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="D85" sqref="D85"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="74.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.7109375" style="3" customWidth="1"/>
+    <col min="4" max="5" width="12.85546875" style="3" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.140625" style="3"/>
+    <col min="7" max="8" width="12.85546875" style="3" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.140625" style="3"/>
+    <col min="10" max="11" width="12.85546875" style="3" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="D3" s="40" t="s">
+        <v>421</v>
+      </c>
+      <c r="E3" s="40"/>
+      <c r="G3" s="40" t="s">
+        <v>422</v>
+      </c>
+      <c r="H3" s="40"/>
+      <c r="J3" s="40" t="s">
+        <v>423</v>
+      </c>
+      <c r="K3" s="40"/>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="D4" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D5" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="38" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D6" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="39">
+        <v>5</v>
+      </c>
+      <c r="G6" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="39">
+        <v>5</v>
+      </c>
+      <c r="J6" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" s="39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="D7" s="38"/>
+      <c r="E7" s="39">
+        <v>0</v>
+      </c>
+      <c r="G7" s="38"/>
+      <c r="H7" s="39">
+        <v>0</v>
+      </c>
+      <c r="J7" s="38"/>
+      <c r="K7" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="D8" s="38">
+        <v>1</v>
+      </c>
+      <c r="E8" s="39">
+        <v>1</v>
+      </c>
+      <c r="G8" s="38">
+        <v>1</v>
+      </c>
+      <c r="H8" s="39">
+        <v>1</v>
+      </c>
+      <c r="J8" s="38">
+        <v>1</v>
+      </c>
+      <c r="K8" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="6"/>
+      <c r="D9" s="38" t="s">
+        <v>449</v>
+      </c>
+      <c r="E9" s="39">
+        <v>5</v>
+      </c>
+      <c r="G9" s="38" t="s">
+        <v>449</v>
+      </c>
+      <c r="H9" s="39">
+        <v>5</v>
+      </c>
+      <c r="J9" s="38" t="s">
+        <v>449</v>
+      </c>
+      <c r="K9" s="39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="7"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="7"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="7"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="6"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="6"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="6"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="D16" s="40" t="s">
+        <v>424</v>
+      </c>
+      <c r="E16" s="40"/>
+      <c r="G16" s="40" t="s">
+        <v>425</v>
+      </c>
+      <c r="H16" s="40"/>
+      <c r="J16" s="40" t="s">
+        <v>426</v>
+      </c>
+      <c r="K16" s="40"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="D17" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="J17" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="K17" s="38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="6"/>
+      <c r="D18" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="J18" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="K18" s="38" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="6"/>
+      <c r="D19" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="39">
+        <v>5</v>
+      </c>
+      <c r="G19" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="H19" s="39">
+        <v>5</v>
+      </c>
+      <c r="J19" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="K19" s="39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="D20" s="38"/>
+      <c r="E20" s="39">
+        <v>0</v>
+      </c>
+      <c r="G20" s="38"/>
+      <c r="H20" s="39">
+        <v>0</v>
+      </c>
+      <c r="J20" s="38"/>
+      <c r="K20" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="D21" s="38">
+        <v>1</v>
+      </c>
+      <c r="E21" s="39">
+        <v>1</v>
+      </c>
+      <c r="G21" s="38">
+        <v>1</v>
+      </c>
+      <c r="H21" s="39">
+        <v>1</v>
+      </c>
+      <c r="J21" s="38">
+        <v>1</v>
+      </c>
+      <c r="K21" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="6"/>
+      <c r="D22" s="38" t="s">
+        <v>449</v>
+      </c>
+      <c r="E22" s="39">
+        <v>5</v>
+      </c>
+      <c r="G22" s="38" t="s">
+        <v>449</v>
+      </c>
+      <c r="H22" s="39">
+        <v>5</v>
+      </c>
+      <c r="J22" s="38" t="s">
+        <v>449</v>
+      </c>
+      <c r="K22" s="39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="7"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="7"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="7"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="6"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B27" s="6"/>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B28" s="6"/>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B29" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="D29" s="40" t="s">
+        <v>427</v>
+      </c>
+      <c r="E29" s="40"/>
+      <c r="G29" s="40" t="s">
+        <v>428</v>
+      </c>
+      <c r="H29" s="40"/>
+      <c r="J29" s="40" t="s">
+        <v>429</v>
+      </c>
+      <c r="K29" s="40"/>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B30" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="D30" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="E30" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="G30" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="H30" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="J30" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="K30" s="38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B31" s="6"/>
+      <c r="D31" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="E31" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="G31" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="H31" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="J31" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="K31" s="38" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B32" s="6"/>
+      <c r="D32" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="E32" s="39">
+        <v>5</v>
+      </c>
+      <c r="G32" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="H32" s="39">
+        <v>5</v>
+      </c>
+      <c r="J32" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="K32" s="39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B33" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="D33" s="38"/>
+      <c r="E33" s="39">
+        <v>0</v>
+      </c>
+      <c r="G33" s="38"/>
+      <c r="H33" s="39">
+        <v>0</v>
+      </c>
+      <c r="J33" s="38"/>
+      <c r="K33" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B34" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="D34" s="38">
+        <v>1</v>
+      </c>
+      <c r="E34" s="39">
+        <v>1</v>
+      </c>
+      <c r="G34" s="38">
+        <v>1</v>
+      </c>
+      <c r="H34" s="39">
+        <v>1</v>
+      </c>
+      <c r="J34" s="38">
+        <v>1</v>
+      </c>
+      <c r="K34" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B35" s="6"/>
+      <c r="D35" s="38" t="s">
+        <v>449</v>
+      </c>
+      <c r="E35" s="39">
+        <v>5</v>
+      </c>
+      <c r="G35" s="38" t="s">
+        <v>449</v>
+      </c>
+      <c r="H35" s="39">
+        <v>5</v>
+      </c>
+      <c r="J35" s="38" t="s">
+        <v>449</v>
+      </c>
+      <c r="K35" s="39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="7"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="7"/>
+      <c r="J36" s="6"/>
+      <c r="K36" s="7"/>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B37" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="J37" s="6"/>
+      <c r="K37" s="6"/>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B38" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="J38" s="6"/>
+      <c r="K38" s="6"/>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="7"/>
+      <c r="J39" s="6"/>
+      <c r="K39" s="7"/>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="7"/>
+      <c r="J40" s="6"/>
+      <c r="K40" s="7"/>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B41" s="6"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="J41" s="7"/>
+      <c r="K41" s="7"/>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B42" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="D42" s="40" t="s">
+        <v>430</v>
+      </c>
+      <c r="E42" s="40"/>
+      <c r="G42" s="40" t="s">
+        <v>431</v>
+      </c>
+      <c r="H42" s="40"/>
+      <c r="J42" s="40" t="s">
+        <v>432</v>
+      </c>
+      <c r="K42" s="40"/>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B43" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="D43" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="E43" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="G43" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="H43" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="J43" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="K43" s="38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B44" s="6"/>
+      <c r="D44" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="E44" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="G44" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="H44" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="J44" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="K44" s="38" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B45" s="6"/>
+      <c r="D45" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="E45" s="39">
+        <v>5</v>
+      </c>
+      <c r="G45" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="H45" s="39">
+        <v>5</v>
+      </c>
+      <c r="J45" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="K45" s="39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B46" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="D46" s="38"/>
+      <c r="E46" s="39">
+        <v>0</v>
+      </c>
+      <c r="G46" s="38"/>
+      <c r="H46" s="39">
+        <v>0</v>
+      </c>
+      <c r="J46" s="38"/>
+      <c r="K46" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B47" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="D47" s="38">
+        <v>1</v>
+      </c>
+      <c r="E47" s="39">
+        <v>1</v>
+      </c>
+      <c r="G47" s="38">
+        <v>1</v>
+      </c>
+      <c r="H47" s="39">
+        <v>1</v>
+      </c>
+      <c r="J47" s="38">
+        <v>1</v>
+      </c>
+      <c r="K47" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B48" s="6"/>
+      <c r="D48" s="38" t="s">
+        <v>449</v>
+      </c>
+      <c r="E48" s="39">
+        <v>5</v>
+      </c>
+      <c r="G48" s="38" t="s">
+        <v>449</v>
+      </c>
+      <c r="H48" s="39">
+        <v>5</v>
+      </c>
+      <c r="J48" s="38" t="s">
+        <v>449</v>
+      </c>
+      <c r="K48" s="39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="7"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="7"/>
+      <c r="J49" s="6"/>
+      <c r="K49" s="7"/>
+    </row>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B50" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="6"/>
+      <c r="J50" s="6"/>
+      <c r="K50" s="6"/>
+    </row>
+    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B51" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="6"/>
+      <c r="J51" s="6"/>
+      <c r="K51" s="6"/>
+    </row>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B52" s="6"/>
+    </row>
+    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B53" s="6"/>
+    </row>
+    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B54" s="6"/>
+    </row>
+    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B55" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="D55" s="40" t="s">
+        <v>433</v>
+      </c>
+      <c r="E55" s="40"/>
+      <c r="G55" s="40" t="s">
+        <v>434</v>
+      </c>
+      <c r="H55" s="40"/>
+      <c r="J55" s="40" t="s">
+        <v>435</v>
+      </c>
+      <c r="K55" s="40"/>
+    </row>
+    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B56" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="D56" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="E56" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="G56" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="H56" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="J56" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="K56" s="38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B57" s="6"/>
+      <c r="D57" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="E57" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="G57" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="H57" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="J57" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="K57" s="38" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B58" s="6"/>
+      <c r="D58" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="E58" s="39">
+        <v>5</v>
+      </c>
+      <c r="G58" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="H58" s="39">
+        <v>5</v>
+      </c>
+      <c r="J58" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="K58" s="39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B59" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="D59" s="38"/>
+      <c r="E59" s="39">
+        <v>0</v>
+      </c>
+      <c r="G59" s="38"/>
+      <c r="H59" s="39">
+        <v>0</v>
+      </c>
+      <c r="J59" s="38"/>
+      <c r="K59" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B60" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="D60" s="38">
+        <v>1</v>
+      </c>
+      <c r="E60" s="39">
+        <v>1</v>
+      </c>
+      <c r="G60" s="38">
+        <v>1</v>
+      </c>
+      <c r="H60" s="39">
+        <v>1</v>
+      </c>
+      <c r="J60" s="38">
+        <v>1</v>
+      </c>
+      <c r="K60" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B61" s="6"/>
+      <c r="D61" s="38" t="s">
+        <v>449</v>
+      </c>
+      <c r="E61" s="39">
+        <v>5</v>
+      </c>
+      <c r="G61" s="38" t="s">
+        <v>449</v>
+      </c>
+      <c r="H61" s="39">
+        <v>5</v>
+      </c>
+      <c r="J61" s="38" t="s">
+        <v>449</v>
+      </c>
+      <c r="K61" s="39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B62" s="6"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="7"/>
+      <c r="G62" s="6"/>
+      <c r="H62" s="7"/>
+      <c r="J62" s="6"/>
+      <c r="K62" s="7"/>
+    </row>
+    <row r="63" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B63" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="D63" s="6"/>
+      <c r="E63" s="6"/>
+      <c r="G63" s="6"/>
+      <c r="H63" s="6"/>
+      <c r="J63" s="6"/>
+      <c r="K63" s="6"/>
+    </row>
+    <row r="64" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B64" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="D64" s="6"/>
+      <c r="E64" s="6"/>
+      <c r="G64" s="6"/>
+      <c r="H64" s="6"/>
+      <c r="J64" s="6"/>
+      <c r="K64" s="6"/>
+    </row>
+    <row r="67" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D67" s="6"/>
+    </row>
+    <row r="68" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B68" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="D68" s="40" t="s">
+        <v>436</v>
+      </c>
+      <c r="E68" s="40"/>
+      <c r="G68" s="40" t="s">
+        <v>437</v>
+      </c>
+      <c r="H68" s="40"/>
+      <c r="J68" s="40" t="s">
+        <v>438</v>
+      </c>
+      <c r="K68" s="40"/>
+    </row>
+    <row r="69" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B69" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="D69" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="E69" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="G69" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="H69" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="J69" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="K69" s="38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="70" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B70" s="6"/>
+      <c r="D70" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="E70" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="G70" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="H70" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="J70" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="K70" s="38" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="71" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B71" s="6"/>
+      <c r="D71" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="E71" s="39">
+        <v>5</v>
+      </c>
+      <c r="G71" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="H71" s="39">
+        <v>5</v>
+      </c>
+      <c r="J71" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="K71" s="39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B72" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="D72" s="38"/>
+      <c r="E72" s="39">
+        <v>0</v>
+      </c>
+      <c r="G72" s="38"/>
+      <c r="H72" s="39">
+        <v>0</v>
+      </c>
+      <c r="J72" s="38"/>
+      <c r="K72" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B73" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="D73" s="38">
+        <v>1</v>
+      </c>
+      <c r="E73" s="39">
+        <v>1</v>
+      </c>
+      <c r="G73" s="38">
+        <v>1</v>
+      </c>
+      <c r="H73" s="39">
+        <v>1</v>
+      </c>
+      <c r="J73" s="38">
+        <v>1</v>
+      </c>
+      <c r="K73" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B74" s="6"/>
+      <c r="D74" s="38" t="s">
+        <v>449</v>
+      </c>
+      <c r="E74" s="39">
+        <v>5</v>
+      </c>
+      <c r="G74" s="38" t="s">
+        <v>449</v>
+      </c>
+      <c r="H74" s="39">
+        <v>5</v>
+      </c>
+      <c r="J74" s="38" t="s">
+        <v>449</v>
+      </c>
+      <c r="K74" s="39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B75" s="6"/>
+      <c r="D75" s="6"/>
+      <c r="E75" s="7"/>
+      <c r="G75" s="6"/>
+      <c r="H75" s="7"/>
+      <c r="J75" s="6"/>
+      <c r="K75" s="7"/>
+    </row>
+    <row r="76" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B76" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="D76" s="6"/>
+      <c r="E76" s="6"/>
+      <c r="G76" s="6"/>
+      <c r="H76" s="6"/>
+      <c r="J76" s="6"/>
+      <c r="K76" s="6"/>
+    </row>
+    <row r="77" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B77" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="D77" s="6"/>
+      <c r="E77" s="6"/>
+      <c r="G77" s="6"/>
+      <c r="H77" s="6"/>
+      <c r="J77" s="6"/>
+      <c r="K77" s="6"/>
+    </row>
+    <row r="78" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D78" s="6"/>
+      <c r="G78" s="7"/>
+      <c r="H78" s="7"/>
+      <c r="J78" s="7"/>
+      <c r="K78" s="7"/>
+    </row>
+    <row r="79" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D79" s="6"/>
+      <c r="G79" s="7"/>
+      <c r="H79" s="7"/>
+      <c r="J79" s="7"/>
+      <c r="K79" s="7"/>
+    </row>
+    <row r="80" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D80" s="6"/>
+    </row>
+    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B81" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D81" s="40" t="s">
+        <v>439</v>
+      </c>
+      <c r="E81" s="40"/>
+      <c r="G81" s="40" t="s">
+        <v>440</v>
+      </c>
+      <c r="H81" s="40"/>
+    </row>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B82" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="D82" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="E82" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="G82" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="H82" s="38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B83" s="6"/>
+      <c r="D83" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="E83" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="G83" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="H83" s="38" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B84" s="6"/>
+      <c r="D84" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="E84" s="39">
+        <v>3</v>
+      </c>
+      <c r="G84" s="38" t="s">
+        <v>164</v>
+      </c>
+      <c r="H84" s="39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B85" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="D85" s="38"/>
+      <c r="E85" s="39">
+        <v>0</v>
+      </c>
+      <c r="G85" s="38"/>
+      <c r="H85" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B86" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="D86" s="38">
+        <v>1</v>
+      </c>
+      <c r="E86" s="39">
+        <v>1</v>
+      </c>
+      <c r="G86" s="38">
+        <v>1</v>
+      </c>
+      <c r="H86" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B87" s="6"/>
+      <c r="D87" s="38" t="s">
+        <v>452</v>
+      </c>
+      <c r="E87" s="39">
+        <v>5</v>
+      </c>
+      <c r="G87" s="38" t="s">
+        <v>452</v>
+      </c>
+      <c r="H87" s="39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B88" s="6"/>
+      <c r="D88" s="6"/>
+      <c r="E88" s="7"/>
+      <c r="G88" s="6"/>
+      <c r="H88" s="7"/>
+    </row>
+    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B89" s="6"/>
+      <c r="D89" s="6"/>
+      <c r="E89" s="6"/>
+      <c r="G89" s="6"/>
+      <c r="H89" s="6"/>
+    </row>
+    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B90" s="6"/>
+      <c r="D90" s="6"/>
+      <c r="E90" s="6"/>
+      <c r="G90" s="6"/>
+      <c r="H90" s="6"/>
+    </row>
+    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B91" s="6"/>
+      <c r="D91" s="6"/>
+    </row>
+    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B92" s="6"/>
+      <c r="D92" s="6"/>
+    </row>
+    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D93" s="6"/>
+    </row>
+    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B94" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="D94" s="40" t="s">
+        <v>441</v>
+      </c>
+      <c r="E94" s="40"/>
+      <c r="G94" s="40" t="s">
+        <v>442</v>
+      </c>
+      <c r="H94" s="40"/>
+    </row>
+    <row r="95" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B95" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="D95" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="E95" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="G95" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="H95" s="38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D96" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="E96" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="G96" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="H96" s="38" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D97" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="E97" s="39">
+        <v>3</v>
+      </c>
+      <c r="G97" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="H97" s="39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B98" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="D98" s="38"/>
+      <c r="E98" s="39">
+        <v>0</v>
+      </c>
+      <c r="G98" s="38"/>
+      <c r="H98" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B99" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="D99" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="E99" s="39">
+        <v>3</v>
+      </c>
+      <c r="G99" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="H99" s="39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="100" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D100" s="38" t="s">
+        <v>451</v>
+      </c>
+      <c r="E100" s="39">
+        <v>5</v>
+      </c>
+      <c r="G100" s="38" t="s">
+        <v>451</v>
+      </c>
+      <c r="H100" s="39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D101" s="38" t="s">
+        <v>450</v>
+      </c>
+      <c r="E101" s="39">
+        <v>5</v>
+      </c>
+      <c r="G101" s="38" t="s">
+        <v>450</v>
+      </c>
+      <c r="H101" s="39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="102" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D102" s="6"/>
+    </row>
+    <row r="103" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D103" s="6"/>
+    </row>
+    <row r="104" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D104" s="6"/>
+    </row>
+    <row r="105" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B105" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="D105" s="40" t="s">
+        <v>443</v>
+      </c>
+      <c r="E105" s="40"/>
+      <c r="G105" s="40" t="s">
+        <v>444</v>
+      </c>
+      <c r="H105" s="40"/>
+    </row>
+    <row r="106" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B106" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="D106" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="E106" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="G106" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="H106" s="38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="107" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D107" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="E107" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="G107" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="H107" s="38" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="108" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D108" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="E108" s="39">
+        <v>5</v>
+      </c>
+      <c r="G108" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="H108" s="39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="109" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B109" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="D109" s="38"/>
+      <c r="E109" s="39">
+        <v>0</v>
+      </c>
+      <c r="G109" s="38"/>
+      <c r="H109" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B110" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="D110" s="38">
+        <v>1</v>
+      </c>
+      <c r="E110" s="39">
+        <v>1</v>
+      </c>
+      <c r="G110" s="38">
+        <v>1</v>
+      </c>
+      <c r="H110" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D111" s="38" t="s">
+        <v>449</v>
+      </c>
+      <c r="E111" s="39">
+        <v>5</v>
+      </c>
+      <c r="G111" s="38" t="s">
+        <v>449</v>
+      </c>
+      <c r="H111" s="39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="112" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D112" s="6"/>
+      <c r="E112" s="7"/>
+      <c r="G112" s="6"/>
+      <c r="H112" s="7"/>
+    </row>
+    <row r="113" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D113" s="6"/>
+      <c r="E113" s="6"/>
+      <c r="G113" s="6"/>
+      <c r="H113" s="6"/>
+    </row>
+    <row r="114" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D114" s="6"/>
+      <c r="E114" s="6"/>
+      <c r="G114" s="6"/>
+      <c r="H114" s="6"/>
+    </row>
+    <row r="117" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B117" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D117" s="40" t="s">
+        <v>445</v>
+      </c>
+      <c r="E117" s="40"/>
+      <c r="G117" s="40" t="s">
+        <v>446</v>
+      </c>
+      <c r="H117" s="40"/>
+    </row>
+    <row r="118" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B118" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="D118" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="E118" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="G118" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="H118" s="38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="119" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D119" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="E119" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="G119" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="H119" s="38" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="120" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D120" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="E120" s="39">
+        <v>5</v>
+      </c>
+      <c r="G120" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="H120" s="39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="121" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B121" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="D121" s="38"/>
+      <c r="E121" s="39">
+        <v>0</v>
+      </c>
+      <c r="G121" s="38"/>
+      <c r="H121" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B122" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="D122" s="38">
+        <v>1</v>
+      </c>
+      <c r="E122" s="39">
+        <v>1</v>
+      </c>
+      <c r="G122" s="38">
+        <v>1</v>
+      </c>
+      <c r="H122" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D123" s="38" t="s">
+        <v>449</v>
+      </c>
+      <c r="E123" s="39">
+        <v>5</v>
+      </c>
+      <c r="G123" s="38" t="s">
+        <v>449</v>
+      </c>
+      <c r="H123" s="39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="124" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D124" s="6"/>
+      <c r="E124" s="7"/>
+      <c r="G124" s="6"/>
+      <c r="H124" s="7"/>
+    </row>
+    <row r="125" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D125" s="6"/>
+      <c r="E125" s="6"/>
+      <c r="G125" s="6"/>
+      <c r="H125" s="6"/>
+    </row>
+    <row r="126" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D126" s="6"/>
+      <c r="E126" s="6"/>
+      <c r="G126" s="6"/>
+      <c r="H126" s="6"/>
+    </row>
+    <row r="130" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B130" s="11" t="s">
+        <v>420</v>
+      </c>
+      <c r="C130" s="12"/>
+      <c r="D130" s="41" t="s">
+        <v>447</v>
+      </c>
+      <c r="E130" s="41"/>
+    </row>
+    <row r="131" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B131" s="11" t="s">
+        <v>393</v>
+      </c>
+      <c r="C131" s="12"/>
+      <c r="D131" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="E131" s="39" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="132" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B132" s="12"/>
+      <c r="C132" s="12"/>
+      <c r="D132" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="E132" s="39" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="133" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B133" s="12"/>
+      <c r="C133" s="12"/>
+      <c r="D133" s="39" t="s">
+        <v>165</v>
+      </c>
+      <c r="E133" s="39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="134" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B134" s="12"/>
+      <c r="C134" s="12"/>
+      <c r="D134" s="39"/>
+      <c r="E134" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B135" s="12"/>
+      <c r="C135" s="12"/>
+      <c r="D135" s="39" t="s">
+        <v>166</v>
+      </c>
+      <c r="E135" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C136" s="12"/>
+      <c r="D136" s="39" t="s">
+        <v>448</v>
+      </c>
+      <c r="E136" s="39">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="27">
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="J42:K42"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="J55:K55"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="G68:H68"/>
+    <mergeCell ref="J68:K68"/>
+    <mergeCell ref="D117:E117"/>
+    <mergeCell ref="G117:H117"/>
+    <mergeCell ref="D130:E130"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="G81:H81"/>
+    <mergeCell ref="D94:E94"/>
+    <mergeCell ref="G94:H94"/>
+    <mergeCell ref="D105:E105"/>
+    <mergeCell ref="G105:H105"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>